<commit_message>
actually that's final draft of project
</commit_message>
<xml_diff>
--- a/project/план.xlsx
+++ b/project/план.xlsx
@@ -215,7 +215,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="204"/>
@@ -522,12 +522,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -648,33 +656,33 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -988,34 +996,34 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="171" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>